<commit_message>
Updated pin mapping list
</commit_message>
<xml_diff>
--- a/ETAG3_PINS.xlsx
+++ b/ETAG3_PINS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jay\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jay\Desktop\GEN3_RFID\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="116">
   <si>
     <t>Pin #</t>
   </si>
@@ -312,6 +312,66 @@
   </si>
   <si>
     <t>TC2</t>
+  </si>
+  <si>
+    <t>0-RX</t>
+  </si>
+  <si>
+    <t>1-TX</t>
+  </si>
+  <si>
+    <t>SERIAL5</t>
+  </si>
+  <si>
+    <t>AIN18</t>
+  </si>
+  <si>
+    <t>TC1</t>
+  </si>
+  <si>
+    <t>AIN19</t>
+  </si>
+  <si>
+    <t>ECI</t>
+  </si>
+  <si>
+    <t>SCOM5PAD3</t>
+  </si>
+  <si>
+    <t>SCOM5PAD2</t>
+  </si>
+  <si>
+    <t>SCOM0PAD2+</t>
+  </si>
+  <si>
+    <t>SCOM0PAD3+</t>
+  </si>
+  <si>
+    <t>*Incorrect in the schematic as SCOM2PAD2</t>
+  </si>
+  <si>
+    <t>*Incorrect in the schematic as SCOM2PAD3</t>
+  </si>
+  <si>
+    <t>Int?</t>
+  </si>
+  <si>
+    <t>SERCOM5PAD2</t>
+  </si>
+  <si>
+    <t>USBDM</t>
+  </si>
+  <si>
+    <t>USBDP</t>
+  </si>
+  <si>
+    <t>SERCOM3PAD2</t>
+  </si>
+  <si>
+    <t>SERCOM3PAD3</t>
+  </si>
+  <si>
+    <t>SERCOM5PAD3</t>
   </si>
 </sst>
 </file>
@@ -365,14 +425,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,22 +756,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" customWidth="1"/>
-    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="7" max="8" width="9.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -725,16 +796,19 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>74</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -753,11 +827,12 @@
       <c r="F2" t="s">
         <v>95</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -776,561 +851,719 @@
       <c r="F3" t="s">
         <v>95</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>9</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="1"/>
+      <c r="K13" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" t="s">
+        <v>105</v>
+      </c>
+      <c r="F16" t="s">
+        <v>100</v>
+      </c>
+      <c r="H16">
+        <v>10</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>28</v>
       </c>
-      <c r="H17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E17" t="s">
+        <v>106</v>
+      </c>
+      <c r="F17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17">
+        <v>11</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="1"/>
+      <c r="K20" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>23</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="1"/>
+      <c r="K21" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>24</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="1"/>
+      <c r="K22" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>25</v>
       </c>
-      <c r="H23" s="1">
+      <c r="I23" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>26</v>
       </c>
-      <c r="H24" s="1">
+      <c r="I24" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>27</v>
       </c>
-      <c r="H25" s="1">
+      <c r="I25" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>29</v>
       </c>
-      <c r="H26" s="1">
+      <c r="I26" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>30</v>
       </c>
-      <c r="H27" s="1">
+      <c r="I27" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>31</v>
       </c>
-      <c r="H28" s="1">
+      <c r="I28" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>32</v>
       </c>
-      <c r="H29" s="1">
+      <c r="I29" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>33</v>
       </c>
-      <c r="H30" s="1">
+      <c r="I30" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>34</v>
       </c>
-      <c r="H31" s="1"/>
-      <c r="J31" t="s">
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>35</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J32" s="1"/>
+      <c r="K32" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>36</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J33" t="s">
+      <c r="J33" s="1"/>
+      <c r="K33" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>37</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" t="s">
+        <v>110</v>
+      </c>
+      <c r="E34" t="s">
+        <v>111</v>
+      </c>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>38</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35" t="s">
+        <v>115</v>
+      </c>
+      <c r="E35" t="s">
+        <v>112</v>
+      </c>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>39</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>40</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>41</v>
       </c>
-      <c r="H38" s="1"/>
-      <c r="I38" s="2" t="s">
+      <c r="C38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" t="s">
+        <v>103</v>
+      </c>
+      <c r="H38">
+        <v>6</v>
+      </c>
+      <c r="I38" s="1"/>
+      <c r="J38" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="J38" s="3" t="s">
+      <c r="K38" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>42</v>
       </c>
-      <c r="H39" s="1"/>
-      <c r="I39" s="2" t="s">
+      <c r="C39" t="s">
+        <v>102</v>
+      </c>
+      <c r="D39" t="s">
+        <v>104</v>
+      </c>
+      <c r="H39">
+        <v>7</v>
+      </c>
+      <c r="I39" s="1"/>
+      <c r="J39" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="J39" s="3" t="s">
+      <c r="K39" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>43</v>
       </c>
-      <c r="H40" s="1"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>44</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="I41" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>45</v>
       </c>
-      <c r="H42" s="1"/>
-      <c r="J42" t="s">
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>8</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>46</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>47</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>48</v>
       </c>
-      <c r="I46" s="1" t="s">
+      <c r="J46" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K46" s="1"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>49</v>
       </c>
-      <c r="I47" s="1" t="s">
+      <c r="J47" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K47" s="1"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>50</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="I48" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>51</v>
       </c>
-      <c r="H49" s="1"/>
-      <c r="J49" t="s">
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J52" t="s">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K50" s="1"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K51" s="1"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K52" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J53" s="4" t="s">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K53" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J54" s="4" t="s">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K54" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J55" s="4" t="s">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K55" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J56" s="4" t="s">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K56" s="4" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>